<commit_message>
Fix datasets and models
</commit_message>
<xml_diff>
--- a/data/vanthoff/Chen_NatCHem_2015_gBL.xlsx
+++ b/data/vanthoff/Chen_NatCHem_2015_gBL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/cromain_ic_ac_uk/Documents/01-Research/Data/TROPIC/vant_Hoff/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexganose/dev/src/tropic/data/vanthoff/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{DF6E7DBF-8118-49E1-B165-1E692BCFC744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39AABE61-A6F5-45A1-91B1-00CAE4F3E8C9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB2E066-4160-DB4B-AFCD-EE0B37D8EEC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C9FD66C6-8DEC-424D-B28B-01FA890DA8A8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15720" xr2:uid="{C9FD66C6-8DEC-424D-B28B-01FA890DA8A8}"/>
   </bookViews>
   <sheets>
     <sheet name="bBL" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>DOI</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>R.Ln([M]eq)</t>
-  </si>
-  <si>
-    <t>DH</t>
   </si>
   <si>
     <t>Comments</t>
@@ -90,9 +87,6 @@
   </si>
   <si>
     <t>Conversion (%)</t>
-  </si>
-  <si>
-    <t>DS</t>
   </si>
   <si>
     <t>10.1038/nchem.2391</t>
@@ -189,7 +183,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -198,29 +192,17 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1253,16 +1235,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2157410</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>341310</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>96837</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>53975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1607,41 +1589,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B164179-3FC5-4BEE-96F0-6C0DC550EC27}">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="E18" sqref="E18:G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" customWidth="1"/>
+    <col min="1" max="1" width="35.83203125" customWidth="1"/>
     <col min="2" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" customWidth="1"/>
-    <col min="8" max="9" width="13.7109375" customWidth="1"/>
-    <col min="10" max="10" width="36.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" customWidth="1"/>
+    <col min="8" max="9" width="13.6640625" customWidth="1"/>
+    <col min="10" max="10" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>4</v>
@@ -1651,14 +1633,14 @@
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="6">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
         <v>10</v>
       </c>
       <c r="C2">
@@ -1668,7 +1650,7 @@
         <f>C2+273.15</f>
         <v>258.14999999999998</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2">
         <f>1/D2</f>
         <v>3.8737168312996321E-3</v>
       </c>
@@ -1680,12 +1662,11 @@
         <v>18.655752147509574</v>
       </c>
       <c r="J2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B3">
         <v>10</v>
       </c>
       <c r="C3">
@@ -1695,7 +1676,7 @@
         <f t="shared" ref="D3:D5" si="0">C3+273.15</f>
         <v>253.14999999999998</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3">
         <f t="shared" ref="E3:E5" si="1">1/D3</f>
         <v>3.9502271380604387E-3</v>
       </c>
@@ -1707,9 +1688,8 @@
         <v>18.350452186686567</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B4">
         <v>10</v>
       </c>
       <c r="C4">
@@ -1719,7 +1699,7 @@
         <f t="shared" si="0"/>
         <v>248.14999999999998</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4">
         <f t="shared" si="1"/>
         <v>4.0298206729800527E-3</v>
       </c>
@@ -1731,282 +1711,102 @@
         <v>17.985867635341712</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15">
+    <row r="5" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5"/>
+      <c r="B5">
         <v>10</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5">
         <v>-30</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
         <v>243.14999999999998</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5">
         <f t="shared" si="1"/>
         <v>4.1126876413736376E-3</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8">
+      <c r="F5"/>
+      <c r="G5">
         <v>8</v>
       </c>
       <c r="H5">
         <f t="shared" si="2"/>
         <v>17.288476977526155</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
+    <row r="9" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="6"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
+    <row r="13" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="6"/>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13"/>
+      <c r="P13"/>
     </row>
-    <row r="9" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J14" s="5"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="6"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-    </row>
-    <row r="13" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-    </row>
-    <row r="17" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="G24" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="G25" t="s">
-        <v>10</v>
-      </c>
+    <row r="17" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
+      <c r="P17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>